<commit_message>
added readme, final changes on report and gui, add test folder
</commit_message>
<xml_diff>
--- a/code/predictions.xlsx
+++ b/code/predictions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,154 +458,176 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>lungaca122.jpeg</t>
+          <t>colonca15.jpeg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lung Adenocarcinoma</t>
+          <t>Colon Adenocarcinoma</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>98.87%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/test/lungaca122.jpeg</t>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/colonca15.jpeg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>lungaca174.jpeg</t>
+          <t>colonca22.jpeg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lung Adenocarcinoma</t>
+          <t>Colon Adenocarcinoma</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>99.99%</t>
+          <t>94.08%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/test/lungaca174.jpeg</t>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/colonca22.jpeg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lungaca275.jpeg</t>
+          <t>colonca39.jpeg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lung Adenocarcinoma</t>
+          <t>Colon Adenocarcinoma</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>98.69%</t>
+          <t>94.24%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/test/lungaca275.jpeg</t>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/colonca39.jpeg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>lungn17.jpeg</t>
+          <t>lungaca122.jpeg</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lung Benign Tissue</t>
+          <t>Lung Adenocarcinoma</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>98.87%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/test/lungn17.jpeg</t>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/lungaca122.jpeg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>lungn135.jpeg</t>
+          <t>lungaca174.jpeg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lung Benign Tissue</t>
+          <t>Lung Adenocarcinoma</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>99.99%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/test/lungn135.jpeg</t>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/lungaca174.jpeg</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>lungscc315.jpeg</t>
+          <t>lungaca275.jpeg</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lung Squamous Cell Carcinoma</t>
+          <t>Lung Adenocarcinoma</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>98.69%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/test/lungscc315.jpeg</t>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/lungaca275.jpeg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>lungscc315.jpeg</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Lung Squamous Cell Carcinoma</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/lungscc315.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>lungscc317.jpeg</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Lung Squamous Cell Carcinoma</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>100.0%</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/test/lungscc317.jpeg</t>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>L:/!school/!uni/!classes/sem2-2023/software technology/assignments/assignment 2/images for test/lungscc317.jpeg</t>
         </is>
       </c>
     </row>

</xml_diff>